<commit_message>
:sparkles: Classificatore su aumentato
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\OneDrive\Documenti\GitHub\FoodX-251_Classification\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F9BA40-EE21-4C6C-B063-E33E6C6A1F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE25E69-C6A9-4FB5-90A7-9EC0DE8D1797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Type</t>
   </si>
@@ -84,22 +84,19 @@
     <t>Estrazione Feature SIFT</t>
   </si>
   <si>
-    <t>5021 (20 Per Classe)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estrazione Feature MobileNetV2 </t>
-  </si>
-  <si>
-    <t>5022 (20 Per Classe)</t>
   </si>
   <si>
     <t>Estrazione Feature MobileNetV3</t>
   </si>
   <si>
-    <t>5023 (20 Per Classe)</t>
+    <t>knn (Dist = cosine; NumNeigh = 51)</t>
   </si>
   <si>
-    <t>knn (Dist = cosine; NumNeigh = 51)</t>
+    <t>knn (Dist = cosine; NumNeigh = 31)</t>
+  </si>
+  <si>
+    <t>Estrazione Feature MobileNetV3 Degradato</t>
   </si>
 </sst>
 </file>
@@ -675,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +785,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>7</v>
@@ -815,10 +812,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>7</v>
@@ -845,13 +842,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
@@ -868,21 +865,49 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <v>33354</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="14"/>
-      <c r="K7"/>
+      <c r="I7" s="3">
+        <v>0.24679000000000001</v>
+      </c>
+      <c r="K7">
+        <v>0.49291299999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <v>33355</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="14"/>
-      <c r="K8"/>
+      <c r="I8" s="3">
+        <v>0.18784390000000001</v>
+      </c>
+      <c r="K8">
+        <v>0.39986659000000002</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">

</xml_diff>

<commit_message>
:construction: Modo per scegliere background
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\OneDrive\Documenti\GitHub\FoodX-251_Classification\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C5E044-7CEE-42DF-81FE-38E205E15E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B30EB4B-6C0D-4897-86F6-BF0436302771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
   <si>
     <t>Type</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>AlexNet (4096)</t>
+  </si>
+  <si>
+    <t>ResNet (2048)</t>
+  </si>
+  <si>
+    <t>SIFT (feat = 10, im = 300, k = 128)</t>
+  </si>
+  <si>
+    <t>Color + LBP</t>
   </si>
 </sst>
 </file>
@@ -307,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -360,6 +369,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -830,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="L18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,24 +868,24 @@
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="20" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="20" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1849,42 +1861,96 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="B27" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="14">
+        <v>570</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
+      <c r="I27" s="15">
+        <v>3</v>
+      </c>
+      <c r="J27" s="13">
+        <v>0.24512</v>
+      </c>
+      <c r="K27" s="14">
+        <v>0.48598999999999998</v>
+      </c>
+      <c r="L27" s="14">
+        <v>0.18309</v>
+      </c>
+      <c r="M27" s="14">
+        <v>0.37685000000000002</v>
+      </c>
       <c r="N27" s="14"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
+      <c r="B28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="14">
+        <v>570</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="14">
+        <v>48</v>
+      </c>
+      <c r="I28" s="15">
+        <v>1</v>
+      </c>
+      <c r="J28" s="13">
+        <v>0.18209</v>
+      </c>
+      <c r="K28" s="14">
+        <v>0.35792000000000002</v>
+      </c>
+      <c r="L28" s="14">
+        <v>0.12964000000000001</v>
+      </c>
+      <c r="M28" s="14">
+        <v>0.26588000000000001</v>
+      </c>
       <c r="N28" s="14"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="12"/>
+      <c r="B29" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="15"/>
-      <c r="J29" s="13"/>
+      <c r="J29" s="20"/>
       <c r="K29" s="14"/>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
@@ -1894,7 +1960,15 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -1909,31 +1983,71 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
+      <c r="B31" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="14">
+        <v>69</v>
+      </c>
+      <c r="G31" s="14">
+        <v>383</v>
+      </c>
       <c r="H31" s="14"/>
       <c r="I31" s="15"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
+      <c r="J31" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="K31" s="14">
+        <v>2.6009999999999998E-2</v>
+      </c>
+      <c r="L31" s="14">
+        <v>4.2519999999999997E-3</v>
+      </c>
+      <c r="M31" s="14">
+        <v>2.2089999999999999E-2</v>
+      </c>
       <c r="N31" s="14"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="B32" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="14">
+        <v>69</v>
+      </c>
+      <c r="G32" s="14">
+        <v>383</v>
+      </c>
       <c r="H32" s="14"/>
       <c r="I32" s="15"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
+      <c r="J32" s="13">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K32" s="14">
+        <v>3.6601000000000002E-2</v>
+      </c>
+      <c r="L32" s="14">
+        <v>5.2500000000000003E-3</v>
+      </c>
+      <c r="M32" s="14">
+        <v>2.784E-2</v>
+      </c>
+      <c r="N32" s="19"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -4497,6 +4611,18 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J1:J9 J10:K21 J24:K1048576">
     <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J21 J24:J1048576">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4519,8 +4645,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J21 J24:J1048576">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="K1:K21 K24:K1048576">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4545,18 +4671,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:K9 K2">
     <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K21 K24:K1048576">
-    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
:art: Mantenimento delle proporzioni
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\OneDrive\Documenti\GitHub\FoodX-251_Classification\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B30EB4B-6C0D-4897-86F6-BF0436302771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFAE8CC-36A9-4799-80FA-613B0E57D176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="58">
   <si>
     <t>Type</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Color + LBP</t>
+  </si>
+  <si>
+    <t>Mantengo le proporzioni</t>
   </si>
 </sst>
 </file>
@@ -316,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,6 +385,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +870,7 @@
     <col min="14" max="14" width="42.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
@@ -887,7 +893,7 @@
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -931,7 +937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -963,7 +969,7 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -995,7 +1001,7 @@
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1027,7 +1033,7 @@
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1059,7 +1065,7 @@
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1086,10 +1092,10 @@
       <c r="J7" s="13">
         <v>0.24679000000000001</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="24">
         <v>0.49291299999999999</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="24">
         <v>0.18784390000000001</v>
       </c>
       <c r="M7" s="14">
@@ -1099,7 +1105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1137,7 +1143,7 @@
       </c>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1176,8 +1182,9 @@
         <v>0.22286</v>
       </c>
       <c r="N9" s="14"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1217,7 +1224,7 @@
       </c>
       <c r="N10" s="14"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1259,7 +1266,7 @@
       </c>
       <c r="N11" s="14"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1299,7 +1306,7 @@
       </c>
       <c r="N12" s="14"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1341,7 +1348,7 @@
       </c>
       <c r="N13" s="14"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1381,7 +1388,7 @@
       </c>
       <c r="N14" s="14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1421,7 +1428,7 @@
       </c>
       <c r="N15" s="14"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2053,31 +2060,79 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
+      <c r="B33" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="14">
+        <v>180</v>
+      </c>
+      <c r="G33" s="14">
+        <v>385</v>
+      </c>
       <c r="H33" s="14"/>
       <c r="I33" s="15"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
+      <c r="J33" s="13">
+        <v>0.27446999999999999</v>
+      </c>
+      <c r="K33" s="14">
+        <v>0.53234899999999996</v>
+      </c>
+      <c r="L33" s="14">
+        <v>0.20018</v>
+      </c>
+      <c r="M33" s="14">
+        <v>0.40244999999999997</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
+      <c r="B34" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="14">
+        <v>180</v>
+      </c>
+      <c r="G34" s="14">
+        <v>385</v>
+      </c>
+      <c r="H34" s="14">
+        <v>120</v>
+      </c>
+      <c r="I34" s="15">
+        <v>1</v>
+      </c>
+      <c r="J34" s="13">
+        <v>0.16649</v>
+      </c>
+      <c r="K34" s="14">
+        <v>0.34166999999999997</v>
+      </c>
+      <c r="L34" s="14">
+        <v>0.11589000000000001</v>
+      </c>
+      <c r="M34" s="14">
+        <v>0.2387</v>
+      </c>
+      <c r="N34" s="14" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">

</xml_diff>